<commit_message>
change excel to py
</commit_message>
<xml_diff>
--- a/backend/resource/neo4j2.xlsx
+++ b/backend/resource/neo4j2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="room" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2082" uniqueCount="864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2087" uniqueCount="860">
   <si>
     <t>总馆北区</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2756,114 +2756,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>参观讲解服务</t>
-  </si>
-  <si>
-    <t>参观讲解服务</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>少年儿童馆</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>触摸屏阅读</t>
-  </si>
-  <si>
-    <r>
-      <t>设有触摸屏</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>台，触摸屏系统集成了报刊、连环画、年画、国图瑰宝、千家诗和少儿游戏六部分内容。报刊包括</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>35</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>种少儿期刊和</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>200</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>种电子报纸；连环画含</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>300</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10.5"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>余种经典作品；“国图瑰宝”含敦煌遗书、赵城金藏、永乐大典、四库全书等经典数字化资源</t>
-    </r>
-  </si>
-  <si>
-    <t>周末故事会、儿童读物与影展、低幼悦读会等形式多样、内容丰富与读书相关的主题活动</t>
-  </si>
-  <si>
-    <t>举办主题活动</t>
-  </si>
-  <si>
-    <t>举办主题活动</t>
-    <rPh sb="0" eb="1">
-      <t>ju ban</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>zhu ti huo dong</t>
-    </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -2924,16 +2817,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>周一至周五</t>
-    <rPh sb="0" eb="1">
-      <t>zhou yi zhi</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>zhou wu</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>周末开放日期</t>
     <rPh sb="0" eb="1">
       <t>zhou mo</t>
@@ -2991,19 +2874,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>周二至周五</t>
-    <rPh sb="0" eb="1">
-      <t>zhou yi zhi</t>
-    </rPh>
-    <rPh sb="1" eb="2">
-      <t>er</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>zhou wu</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>总馆南区</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3017,10 +2887,6 @@
   </si>
   <si>
     <t>24小时（自助）还书处</t>
-  </si>
-  <si>
-    <t>触摸屏阅读</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>证件</t>
@@ -4277,6 +4143,42 @@
   </si>
   <si>
     <t>中文图书阅览区</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>活动</t>
+    <rPh sb="0" eb="1">
+      <t>huo dong</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工作日时间</t>
+    <rPh sb="0" eb="1">
+      <t>gong zuo ri shi jian</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>周末故事会</t>
+  </si>
+  <si>
+    <t>儿童读物与影展</t>
+  </si>
+  <si>
+    <t>低幼悦读会</t>
+  </si>
+  <si>
+    <t>周一至周日</t>
+    <rPh sb="0" eb="1">
+      <t>zhou yi zhi</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>zhou wu</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>ri</t>
+    </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4919,7 +4821,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="AB8" sqref="AB8"/>
     </sheetView>
   </sheetViews>
@@ -5041,12 +4943,12 @@
         <v>586</v>
       </c>
       <c r="AE1" t="s">
-        <v>804</v>
+        <v>794</v>
       </c>
     </row>
     <row r="2" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>675</v>
+        <v>665</v>
       </c>
       <c r="B2" t="s">
         <v>208</v>
@@ -5061,7 +4963,7 @@
         <v>40</v>
       </c>
       <c r="F2" s="29" t="s">
-        <v>677</v>
+        <v>667</v>
       </c>
       <c r="G2" t="s">
         <v>90</v>
@@ -5109,7 +5011,7 @@
         <v>0</v>
       </c>
       <c r="V2" t="s">
-        <v>676</v>
+        <v>666</v>
       </c>
       <c r="W2" t="s">
         <v>579</v>
@@ -5163,13 +5065,13 @@
         <v>557</v>
       </c>
       <c r="Z5" t="s">
-        <v>845</v>
+        <v>835</v>
       </c>
       <c r="AA5" t="s">
-        <v>847</v>
+        <v>837</v>
       </c>
       <c r="AB5" t="s">
-        <v>856</v>
+        <v>846</v>
       </c>
       <c r="AC5" t="s">
         <v>568</v>
@@ -5177,10 +5079,10 @@
     </row>
     <row r="6" spans="1:31" ht="75" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>863</v>
+        <v>853</v>
       </c>
       <c r="B6" t="s">
-        <v>679</v>
+        <v>669</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>
@@ -5240,7 +5142,7 @@
         <v>502</v>
       </c>
       <c r="V6" t="s">
-        <v>680</v>
+        <v>670</v>
       </c>
       <c r="W6" t="s">
         <v>579</v>
@@ -5249,13 +5151,13 @@
         <v>557</v>
       </c>
       <c r="Z6" t="s">
-        <v>845</v>
+        <v>835</v>
       </c>
       <c r="AA6" t="s">
-        <v>847</v>
+        <v>837</v>
       </c>
       <c r="AB6" t="s">
-        <v>856</v>
+        <v>846</v>
       </c>
       <c r="AC6" t="s">
         <v>568</v>
@@ -5269,7 +5171,7 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>681</v>
+        <v>671</v>
       </c>
       <c r="B7" t="s">
         <v>371</v>
@@ -5284,13 +5186,13 @@
         <v>557</v>
       </c>
       <c r="Z7" t="s">
-        <v>845</v>
+        <v>835</v>
       </c>
       <c r="AA7" t="s">
-        <v>847</v>
+        <v>837</v>
       </c>
       <c r="AB7" t="s">
-        <v>856</v>
+        <v>846</v>
       </c>
       <c r="AC7" t="s">
         <v>568</v>
@@ -5298,22 +5200,22 @@
     </row>
     <row r="8" spans="1:31" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="37" t="s">
-        <v>724</v>
+        <v>714</v>
       </c>
       <c r="B8" t="s">
-        <v>688</v>
+        <v>678</v>
       </c>
       <c r="C8" t="s">
         <v>120</v>
       </c>
       <c r="D8" s="29" t="s">
-        <v>689</v>
+        <v>679</v>
       </c>
       <c r="E8" t="s">
         <v>40</v>
       </c>
       <c r="F8" s="29" t="s">
-        <v>690</v>
+        <v>680</v>
       </c>
       <c r="G8" t="s">
         <v>91</v>
@@ -5352,22 +5254,22 @@
         <v>91</v>
       </c>
       <c r="U8" t="s">
-        <v>698</v>
+        <v>688</v>
       </c>
       <c r="V8" t="s">
-        <v>700</v>
+        <v>690</v>
       </c>
       <c r="X8" s="2" t="s">
         <v>557</v>
       </c>
       <c r="Z8" t="s">
-        <v>845</v>
+        <v>835</v>
       </c>
       <c r="AA8" t="s">
-        <v>847</v>
+        <v>837</v>
       </c>
       <c r="AB8" t="s">
-        <v>856</v>
+        <v>846</v>
       </c>
       <c r="AC8" t="s">
         <v>568</v>
@@ -5375,7 +5277,7 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>716</v>
+        <v>706</v>
       </c>
       <c r="B9" t="s">
         <v>414</v>
@@ -5412,15 +5314,15 @@
         <v>91</v>
       </c>
       <c r="U9" t="s">
-        <v>712</v>
+        <v>702</v>
       </c>
       <c r="V9" t="s">
-        <v>718</v>
+        <v>708</v>
       </c>
     </row>
     <row r="10" spans="1:31" ht="90" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>717</v>
+        <v>707</v>
       </c>
       <c r="B10" t="s">
         <v>415</v>
@@ -5435,7 +5337,7 @@
         <v>40</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>697</v>
+        <v>687</v>
       </c>
       <c r="G10" t="s">
         <v>90</v>
@@ -5459,22 +5361,22 @@
         <v>93</v>
       </c>
       <c r="U10" t="s">
-        <v>719</v>
+        <v>709</v>
       </c>
       <c r="V10" t="s">
-        <v>682</v>
+        <v>672</v>
       </c>
       <c r="X10" s="2" t="s">
         <v>557</v>
       </c>
       <c r="Z10" t="s">
-        <v>845</v>
+        <v>835</v>
       </c>
       <c r="AA10" t="s">
-        <v>847</v>
+        <v>837</v>
       </c>
       <c r="AB10" t="s">
-        <v>856</v>
+        <v>846</v>
       </c>
       <c r="AC10" t="s">
         <v>568</v>
@@ -5497,13 +5399,13 @@
         <v>557</v>
       </c>
       <c r="Z11" t="s">
-        <v>845</v>
+        <v>835</v>
       </c>
       <c r="AA11" t="s">
-        <v>847</v>
+        <v>837</v>
       </c>
       <c r="AB11" t="s">
-        <v>856</v>
+        <v>846</v>
       </c>
       <c r="AC11" t="s">
         <v>568</v>
@@ -5526,13 +5428,13 @@
         <v>557</v>
       </c>
       <c r="Z12" t="s">
-        <v>845</v>
+        <v>835</v>
       </c>
       <c r="AA12" t="s">
-        <v>847</v>
+        <v>837</v>
       </c>
       <c r="AB12" t="s">
-        <v>856</v>
+        <v>846</v>
       </c>
       <c r="AC12" t="s">
         <v>568</v>
@@ -5555,13 +5457,13 @@
         <v>557</v>
       </c>
       <c r="Z13" t="s">
-        <v>845</v>
+        <v>835</v>
       </c>
       <c r="AA13" t="s">
-        <v>847</v>
+        <v>837</v>
       </c>
       <c r="AB13" t="s">
-        <v>856</v>
+        <v>846</v>
       </c>
       <c r="AC13" t="s">
         <v>568</v>
@@ -5569,7 +5471,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>708</v>
+        <v>698</v>
       </c>
       <c r="B14" t="s">
         <v>407</v>
@@ -5608,22 +5510,22 @@
         <v>91</v>
       </c>
       <c r="U14" t="s">
-        <v>698</v>
+        <v>688</v>
       </c>
       <c r="V14" t="s">
-        <v>699</v>
+        <v>689</v>
       </c>
       <c r="X14" s="2" t="s">
         <v>557</v>
       </c>
       <c r="Z14" t="s">
-        <v>845</v>
+        <v>835</v>
       </c>
       <c r="AA14" t="s">
-        <v>847</v>
+        <v>837</v>
       </c>
       <c r="AB14" t="s">
-        <v>856</v>
+        <v>846</v>
       </c>
       <c r="AC14" t="s">
         <v>568</v>
@@ -5631,7 +5533,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>709</v>
+        <v>699</v>
       </c>
       <c r="B15" t="s">
         <v>407</v>
@@ -5670,22 +5572,22 @@
         <v>91</v>
       </c>
       <c r="U15" t="s">
-        <v>712</v>
+        <v>702</v>
       </c>
       <c r="V15" t="s">
-        <v>699</v>
+        <v>689</v>
       </c>
       <c r="X15" s="2" t="s">
         <v>557</v>
       </c>
       <c r="Z15" t="s">
-        <v>845</v>
+        <v>835</v>
       </c>
       <c r="AA15" t="s">
-        <v>847</v>
+        <v>837</v>
       </c>
       <c r="AB15" t="s">
-        <v>856</v>
+        <v>846</v>
       </c>
       <c r="AC15" t="s">
         <v>568</v>
@@ -5693,7 +5595,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>710</v>
+        <v>700</v>
       </c>
       <c r="B16" t="s">
         <v>420</v>
@@ -5705,7 +5607,7 @@
         <v>121</v>
       </c>
       <c r="E16" t="s">
-        <v>711</v>
+        <v>701</v>
       </c>
       <c r="F16" t="s">
         <v>28</v>
@@ -5726,22 +5628,22 @@
         <v>91</v>
       </c>
       <c r="U16" t="s">
-        <v>713</v>
+        <v>703</v>
       </c>
       <c r="V16" t="s">
-        <v>714</v>
+        <v>704</v>
       </c>
       <c r="X16" s="2" t="s">
         <v>557</v>
       </c>
       <c r="Z16" t="s">
-        <v>845</v>
+        <v>835</v>
       </c>
       <c r="AA16" t="s">
-        <v>847</v>
+        <v>837</v>
       </c>
       <c r="AB16" t="s">
-        <v>856</v>
+        <v>846</v>
       </c>
       <c r="AC16" t="s">
         <v>568</v>
@@ -5790,10 +5692,10 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>691</v>
+        <v>681</v>
       </c>
       <c r="B18" t="s">
-        <v>805</v>
+        <v>795</v>
       </c>
       <c r="C18" t="s">
         <v>124</v>
@@ -5826,10 +5728,10 @@
         <v>91</v>
       </c>
       <c r="U18" t="s">
-        <v>698</v>
+        <v>688</v>
       </c>
       <c r="V18" t="s">
-        <v>701</v>
+        <v>691</v>
       </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
@@ -5934,7 +5836,7 @@
         <v>411</v>
       </c>
       <c r="B24" t="s">
-        <v>696</v>
+        <v>686</v>
       </c>
       <c r="C24" t="s">
         <v>140</v>
@@ -5997,7 +5899,7 @@
         <v>270</v>
       </c>
       <c r="W24" t="s">
-        <v>695</v>
+        <v>685</v>
       </c>
       <c r="AE24">
         <v>1</v>
@@ -6070,10 +5972,10 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>693</v>
+        <v>683</v>
       </c>
       <c r="B26" t="s">
-        <v>692</v>
+        <v>682</v>
       </c>
       <c r="C26" t="s">
         <v>35</v>
@@ -6147,7 +6049,7 @@
         <v>593</v>
       </c>
       <c r="B27" t="s">
-        <v>694</v>
+        <v>684</v>
       </c>
       <c r="C27" t="s">
         <v>35</v>
@@ -6284,7 +6186,7 @@
         <v>270</v>
       </c>
       <c r="W28" t="s">
-        <v>687</v>
+        <v>677</v>
       </c>
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
@@ -6355,7 +6257,7 @@
         <v>270</v>
       </c>
       <c r="W29" t="s">
-        <v>687</v>
+        <v>677</v>
       </c>
       <c r="AE29">
         <v>1</v>
@@ -6363,7 +6265,7 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>704</v>
+        <v>694</v>
       </c>
       <c r="B30" t="s">
         <v>416</v>
@@ -6402,10 +6304,10 @@
         <v>93</v>
       </c>
       <c r="U30" t="s">
-        <v>706</v>
+        <v>696</v>
       </c>
       <c r="V30" t="s">
-        <v>707</v>
+        <v>697</v>
       </c>
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
@@ -6424,10 +6326,10 @@
     </row>
     <row r="32" spans="1:31" ht="45" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="B32" t="s">
-        <v>660</v>
+        <v>650</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>30</v>
@@ -6487,19 +6389,19 @@
         <v>148</v>
       </c>
       <c r="W32" s="2" t="s">
-        <v>655</v>
+        <v>645</v>
       </c>
       <c r="X32" s="2" t="s">
         <v>557</v>
       </c>
       <c r="Z32" t="s">
-        <v>845</v>
+        <v>835</v>
       </c>
       <c r="AA32" s="38" t="s">
+        <v>836</v>
+      </c>
+      <c r="AB32" t="s">
         <v>846</v>
-      </c>
-      <c r="AB32" t="s">
-        <v>856</v>
       </c>
       <c r="AC32" t="s">
         <v>568</v>
@@ -6707,7 +6609,7 @@
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>702</v>
+        <v>692</v>
       </c>
       <c r="B37" t="s">
         <v>405</v>
@@ -6849,7 +6751,7 @@
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>720</v>
+        <v>710</v>
       </c>
       <c r="B39" t="s">
         <v>417</v>
@@ -6899,13 +6801,13 @@
         <v>22</v>
       </c>
       <c r="B40" t="s">
-        <v>824</v>
+        <v>814</v>
       </c>
       <c r="C40" t="s">
         <v>112</v>
       </c>
       <c r="D40" t="s">
-        <v>825</v>
+        <v>815</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>228</v>
@@ -6955,7 +6857,7 @@
         <v>111</v>
       </c>
       <c r="B41" t="s">
-        <v>823</v>
+        <v>813</v>
       </c>
       <c r="C41" t="s">
         <v>112</v>
@@ -7064,7 +6966,7 @@
     </row>
     <row r="43" spans="1:31" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>809</v>
+        <v>799</v>
       </c>
       <c r="B43" t="s">
         <v>403</v>
@@ -7188,7 +7090,7 @@
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>703</v>
+        <v>693</v>
       </c>
       <c r="B45" t="s">
         <v>400</v>
@@ -7395,7 +7297,7 @@
     </row>
     <row r="48" spans="1:31" ht="30" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>705</v>
+        <v>695</v>
       </c>
       <c r="B48" t="s">
         <v>398</v>
@@ -7646,13 +7548,13 @@
     </row>
     <row r="52" spans="1:31" ht="30" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>810</v>
+        <v>800</v>
       </c>
       <c r="B52" t="s">
-        <v>812</v>
+        <v>802</v>
       </c>
       <c r="D52" s="29" t="s">
-        <v>811</v>
+        <v>801</v>
       </c>
       <c r="E52" s="2" t="s">
         <v>228</v>
@@ -8098,7 +8000,7 @@
     </row>
     <row r="59" spans="1:31" ht="30" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>721</v>
+        <v>711</v>
       </c>
       <c r="B59" t="s">
         <v>501</v>
@@ -8149,7 +8051,7 @@
         <v>16</v>
       </c>
       <c r="V59" t="s">
-        <v>722</v>
+        <v>712</v>
       </c>
     </row>
     <row r="60" spans="1:31" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -8720,13 +8622,13 @@
         <v>557</v>
       </c>
       <c r="Z79" s="38" t="s">
-        <v>844</v>
+        <v>834</v>
       </c>
       <c r="AA79" s="38" t="s">
+        <v>836</v>
+      </c>
+      <c r="AB79" t="s">
         <v>846</v>
-      </c>
-      <c r="AB79" t="s">
-        <v>856</v>
       </c>
       <c r="AC79" t="s">
         <v>568</v>
@@ -8806,13 +8708,13 @@
         <v>557</v>
       </c>
       <c r="Z80" s="38" t="s">
-        <v>844</v>
+        <v>834</v>
       </c>
       <c r="AA80" s="38" t="s">
+        <v>836</v>
+      </c>
+      <c r="AB80" t="s">
         <v>846</v>
-      </c>
-      <c r="AB80" t="s">
-        <v>856</v>
       </c>
       <c r="AC80" t="s">
         <v>568</v>
@@ -8892,13 +8794,13 @@
         <v>557</v>
       </c>
       <c r="Z81" s="38" t="s">
-        <v>844</v>
+        <v>834</v>
       </c>
       <c r="AA81" s="38" t="s">
+        <v>836</v>
+      </c>
+      <c r="AB81" t="s">
         <v>846</v>
-      </c>
-      <c r="AB81" t="s">
-        <v>856</v>
       </c>
       <c r="AC81" t="s">
         <v>568</v>
@@ -8978,13 +8880,13 @@
         <v>557</v>
       </c>
       <c r="Z82" s="38" t="s">
-        <v>844</v>
+        <v>834</v>
       </c>
       <c r="AA82" s="38" t="s">
+        <v>836</v>
+      </c>
+      <c r="AB82" t="s">
         <v>846</v>
-      </c>
-      <c r="AB82" t="s">
-        <v>856</v>
       </c>
       <c r="AC82" t="s">
         <v>568</v>
@@ -9061,13 +8963,13 @@
         <v>557</v>
       </c>
       <c r="Z83" s="38" t="s">
-        <v>844</v>
+        <v>834</v>
       </c>
       <c r="AA83" s="38" t="s">
+        <v>836</v>
+      </c>
+      <c r="AB83" t="s">
         <v>846</v>
-      </c>
-      <c r="AB83" t="s">
-        <v>856</v>
       </c>
       <c r="AC83" t="s">
         <v>568</v>
@@ -9090,13 +8992,13 @@
         <v>567</v>
       </c>
       <c r="Z84" t="s">
-        <v>848</v>
+        <v>838</v>
       </c>
       <c r="AA84" t="s">
-        <v>849</v>
+        <v>839</v>
       </c>
       <c r="AB84" t="s">
-        <v>856</v>
+        <v>846</v>
       </c>
       <c r="AC84" t="s">
         <v>569</v>
@@ -9104,22 +9006,22 @@
     </row>
     <row r="85" spans="1:31" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>723</v>
+        <v>713</v>
       </c>
       <c r="B85" t="s">
-        <v>683</v>
+        <v>673</v>
       </c>
       <c r="C85" s="29" t="s">
-        <v>684</v>
+        <v>674</v>
       </c>
       <c r="D85" s="29" t="s">
-        <v>685</v>
+        <v>675</v>
       </c>
       <c r="E85" t="s">
         <v>40</v>
       </c>
       <c r="F85" s="29" t="s">
-        <v>686</v>
+        <v>676</v>
       </c>
       <c r="G85" t="s">
         <v>90</v>
@@ -9170,19 +9072,19 @@
         <v>148</v>
       </c>
       <c r="W85" t="s">
-        <v>687</v>
+        <v>677</v>
       </c>
       <c r="X85" t="s">
         <v>567</v>
       </c>
       <c r="Z85" t="s">
-        <v>848</v>
+        <v>838</v>
       </c>
       <c r="AA85" t="s">
-        <v>849</v>
+        <v>839</v>
       </c>
       <c r="AB85" t="s">
-        <v>856</v>
+        <v>846</v>
       </c>
       <c r="AC85" t="s">
         <v>569</v>
@@ -9193,10 +9095,10 @@
     </row>
     <row r="86" spans="1:31" ht="30" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>657</v>
+        <v>647</v>
       </c>
       <c r="B86" t="s">
-        <v>658</v>
+        <v>648</v>
       </c>
       <c r="C86" s="2" t="s">
         <v>31</v>
@@ -9265,13 +9167,13 @@
         <v>557</v>
       </c>
       <c r="Z86" t="s">
-        <v>845</v>
+        <v>835</v>
       </c>
       <c r="AA86" t="s">
-        <v>847</v>
+        <v>837</v>
       </c>
       <c r="AB86" t="s">
-        <v>856</v>
+        <v>846</v>
       </c>
       <c r="AC86" t="s">
         <v>568</v>
@@ -9300,13 +9202,13 @@
         <v>559</v>
       </c>
       <c r="Z87" t="s">
-        <v>848</v>
+        <v>838</v>
       </c>
       <c r="AA87" t="s">
-        <v>849</v>
+        <v>839</v>
       </c>
       <c r="AB87" t="s">
-        <v>857</v>
+        <v>847</v>
       </c>
       <c r="AC87" t="s">
         <v>570</v>
@@ -9335,13 +9237,13 @@
         <v>558</v>
       </c>
       <c r="Z88" t="s">
+        <v>838</v>
+      </c>
+      <c r="AA88" t="s">
+        <v>839</v>
+      </c>
+      <c r="AB88" t="s">
         <v>848</v>
-      </c>
-      <c r="AA88" t="s">
-        <v>849</v>
-      </c>
-      <c r="AB88" t="s">
-        <v>858</v>
       </c>
       <c r="AC88" t="s">
         <v>571</v>
@@ -9373,13 +9275,13 @@
         <v>561</v>
       </c>
       <c r="Z89" t="s">
-        <v>850</v>
+        <v>840</v>
       </c>
       <c r="AA89" t="s">
-        <v>851</v>
+        <v>841</v>
       </c>
       <c r="AB89" t="s">
-        <v>859</v>
+        <v>849</v>
       </c>
       <c r="AC89" t="s">
         <v>572</v>
@@ -9408,13 +9310,13 @@
         <v>562</v>
       </c>
       <c r="Z90" t="s">
-        <v>852</v>
+        <v>842</v>
       </c>
       <c r="AA90" t="s">
-        <v>853</v>
+        <v>843</v>
       </c>
       <c r="AB90" t="s">
-        <v>860</v>
+        <v>850</v>
       </c>
       <c r="AC90" t="s">
         <v>573</v>
@@ -9443,13 +9345,13 @@
         <v>563</v>
       </c>
       <c r="Z91" t="s">
-        <v>848</v>
+        <v>838</v>
       </c>
       <c r="AA91" t="s">
-        <v>849</v>
+        <v>839</v>
       </c>
       <c r="AB91" t="s">
-        <v>861</v>
+        <v>851</v>
       </c>
       <c r="AC91" t="s">
         <v>574</v>
@@ -9481,13 +9383,13 @@
         <v>565</v>
       </c>
       <c r="Z92" s="28" t="s">
-        <v>854</v>
+        <v>844</v>
       </c>
       <c r="AA92" t="s">
-        <v>855</v>
+        <v>845</v>
       </c>
       <c r="AB92" t="s">
-        <v>862</v>
+        <v>852</v>
       </c>
       <c r="AC92" t="s">
         <v>575</v>
@@ -9535,7 +9437,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>733</v>
+        <v>723</v>
       </c>
       <c r="B1" t="s">
         <v>536</v>
@@ -9543,7 +9445,7 @@
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>732</v>
+        <v>722</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>610</v>
@@ -9551,7 +9453,7 @@
     </row>
     <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
-        <v>734</v>
+        <v>724</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>610</v>
@@ -9559,7 +9461,7 @@
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="29" t="s">
-        <v>735</v>
+        <v>725</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>610</v>
@@ -9622,10 +9524,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>656</v>
+        <v>646</v>
       </c>
       <c r="B4" t="s">
-        <v>834</v>
+        <v>824</v>
       </c>
       <c r="C4" t="s">
         <v>584</v>
@@ -9639,7 +9541,7 @@
         <v>614</v>
       </c>
       <c r="B5" t="s">
-        <v>833</v>
+        <v>823</v>
       </c>
       <c r="C5" t="s">
         <v>585</v>
@@ -9658,8 +9560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9675,16 +9577,16 @@
         <v>514</v>
       </c>
       <c r="D1" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
       <c r="E1" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
       <c r="F1" t="s">
-        <v>643</v>
+        <v>635</v>
       </c>
       <c r="G1" t="s">
-        <v>645</v>
+        <v>637</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -9698,21 +9600,21 @@
         <v>578</v>
       </c>
       <c r="D2" t="s">
-        <v>640</v>
+        <v>859</v>
       </c>
       <c r="E2" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
       <c r="F2" t="s">
-        <v>644</v>
+        <v>636</v>
       </c>
       <c r="G2" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>648</v>
+        <v>639</v>
       </c>
       <c r="B3" t="s">
         <v>373</v>
@@ -9721,21 +9623,21 @@
         <v>577</v>
       </c>
       <c r="D3" t="s">
-        <v>640</v>
+        <v>859</v>
       </c>
       <c r="E3" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
       <c r="F3" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
       <c r="G3" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>649</v>
+        <v>640</v>
       </c>
       <c r="B4" t="s">
         <v>375</v>
@@ -9744,39 +9646,39 @@
         <v>576</v>
       </c>
       <c r="D4" t="s">
-        <v>640</v>
+        <v>859</v>
       </c>
       <c r="E4" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
       <c r="F4" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
       <c r="G4" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>650</v>
+        <v>641</v>
       </c>
       <c r="B5" t="s">
-        <v>715</v>
+        <v>705</v>
       </c>
       <c r="C5" t="s">
         <v>576</v>
       </c>
       <c r="D5" t="s">
-        <v>647</v>
+        <v>859</v>
       </c>
       <c r="E5" t="s">
-        <v>642</v>
+        <v>634</v>
       </c>
       <c r="F5" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
       <c r="G5" t="s">
-        <v>646</v>
+        <v>638</v>
       </c>
     </row>
   </sheetData>
@@ -9824,19 +9726,19 @@
         <v>539</v>
       </c>
       <c r="G1" t="s">
-        <v>725</v>
+        <v>715</v>
       </c>
       <c r="H1" t="s">
-        <v>726</v>
+        <v>716</v>
       </c>
       <c r="I1" t="s">
-        <v>727</v>
+        <v>717</v>
       </c>
       <c r="J1" t="s">
-        <v>728</v>
+        <v>718</v>
       </c>
       <c r="K1" t="s">
-        <v>729</v>
+        <v>719</v>
       </c>
       <c r="L1" t="s">
         <v>616</v>
@@ -9844,34 +9746,34 @@
     </row>
     <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>662</v>
+        <v>652</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>661</v>
+        <v>651</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="8">
         <v>9814446</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>678</v>
+        <v>668</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>284</v>
       </c>
       <c r="I2" t="s">
-        <v>757</v>
+        <v>747</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>663</v>
+        <v>653</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>425</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>793</v>
+        <v>783</v>
       </c>
       <c r="D3" s="8">
         <v>1722826</v>
@@ -9883,10 +9785,10 @@
         <v>284</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>758</v>
+        <v>748</v>
       </c>
       <c r="J3" s="31" t="s">
-        <v>785</v>
+        <v>775</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30" x14ac:dyDescent="0.2">
@@ -9910,7 +9812,7 @@
         <v>1984</v>
       </c>
       <c r="I4" t="s">
-        <v>757</v>
+        <v>747</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -9934,7 +9836,7 @@
         <v>1984</v>
       </c>
       <c r="I5" t="s">
-        <v>757</v>
+        <v>747</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.2">
@@ -9956,7 +9858,7 @@
       </c>
       <c r="G6" s="29"/>
       <c r="I6" t="s">
-        <v>757</v>
+        <v>747</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.2">
@@ -9980,7 +9882,7 @@
         <v>1984</v>
       </c>
       <c r="I7" t="s">
-        <v>757</v>
+        <v>747</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -9995,13 +9897,13 @@
         <v>2337712</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>832</v>
+        <v>822</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>288</v>
       </c>
       <c r="I8" t="s">
-        <v>757</v>
+        <v>747</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="30" x14ac:dyDescent="0.2">
@@ -10016,13 +9918,13 @@
         <v>2337712</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>832</v>
+        <v>822</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>288</v>
       </c>
       <c r="I9" t="s">
-        <v>757</v>
+        <v>747</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.2">
@@ -10037,18 +9939,18 @@
         <v>2337712</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>832</v>
+        <v>822</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>288</v>
       </c>
       <c r="I10" t="s">
-        <v>757</v>
+        <v>747</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>664</v>
+        <v>654</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>608</v>
@@ -10058,13 +9960,13 @@
         <v>676822</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>702</v>
+        <v>692</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>288</v>
       </c>
       <c r="I11" t="s">
-        <v>757</v>
+        <v>747</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="45" x14ac:dyDescent="0.2">
@@ -10079,13 +9981,13 @@
         <v>1214830</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>702</v>
+        <v>692</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>288</v>
       </c>
       <c r="I12" s="38" t="s">
-        <v>756</v>
+        <v>746</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.2">
@@ -10107,7 +10009,7 @@
         <v>1984</v>
       </c>
       <c r="I13" t="s">
-        <v>755</v>
+        <v>745</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.2">
@@ -10123,24 +10025,24 @@
         <v>289</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>665</v>
+        <v>655</v>
       </c>
       <c r="G14" s="29">
         <v>1984</v>
       </c>
       <c r="I14" t="s">
-        <v>659</v>
+        <v>649</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>744</v>
+        <v>734</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>800</v>
+        <v>790</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>794</v>
+        <v>784</v>
       </c>
       <c r="D15" s="8">
         <v>341573</v>
@@ -10155,21 +10057,21 @@
         <v>1910</v>
       </c>
       <c r="I15" s="31" t="s">
-        <v>760</v>
+        <v>750</v>
       </c>
       <c r="J15" s="31" t="s">
-        <v>741</v>
+        <v>731</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="345" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>745</v>
+        <v>735</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>801</v>
+        <v>791</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>753</v>
+        <v>743</v>
       </c>
       <c r="D16" s="8">
         <v>341573</v>
@@ -10184,21 +10086,21 @@
         <v>1954</v>
       </c>
       <c r="I16" s="31" t="s">
-        <v>762</v>
+        <v>752</v>
       </c>
       <c r="J16" s="31" t="s">
-        <v>741</v>
+        <v>731</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="60" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>746</v>
+        <v>736</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>802</v>
+        <v>792</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>792</v>
+        <v>782</v>
       </c>
       <c r="D17" s="8">
         <v>341573</v>
@@ -10213,21 +10115,21 @@
         <v>1910</v>
       </c>
       <c r="I17" s="31" t="s">
-        <v>791</v>
+        <v>781</v>
       </c>
       <c r="J17" s="31" t="s">
-        <v>741</v>
+        <v>731</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>796</v>
+        <v>786</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>797</v>
+        <v>787</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>768</v>
+        <v>758</v>
       </c>
       <c r="D18" s="8">
         <v>183083</v>
@@ -10242,21 +10144,21 @@
         <v>1929</v>
       </c>
       <c r="I18" s="31" t="s">
-        <v>786</v>
+        <v>776</v>
       </c>
       <c r="J18" s="31" t="s">
-        <v>787</v>
+        <v>777</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>796</v>
+        <v>786</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>798</v>
+        <v>788</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>768</v>
+        <v>758</v>
       </c>
       <c r="D19" s="8">
         <v>183083</v>
@@ -10271,10 +10173,10 @@
         <v>1929</v>
       </c>
       <c r="I19" s="31" t="s">
-        <v>786</v>
+        <v>776</v>
       </c>
       <c r="J19" s="31" t="s">
-        <v>787</v>
+        <v>777</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -10297,13 +10199,13 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>789</v>
+        <v>779</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>440</v>
       </c>
       <c r="C21" s="42" t="s">
-        <v>790</v>
+        <v>780</v>
       </c>
       <c r="D21">
         <v>32941</v>
@@ -10318,10 +10220,10 @@
         <v>1929</v>
       </c>
       <c r="I21" s="42" t="s">
-        <v>761</v>
+        <v>751</v>
       </c>
       <c r="J21" t="s">
-        <v>742</v>
+        <v>732</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -10332,7 +10234,7 @@
         <v>442</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>764</v>
+        <v>754</v>
       </c>
       <c r="D22" s="8">
         <v>110430</v>
@@ -10347,18 +10249,18 @@
         <v>1954</v>
       </c>
       <c r="I22" s="31" t="s">
-        <v>754</v>
+        <v>744</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>769</v>
+        <v>759</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>799</v>
+        <v>789</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>770</v>
+        <v>760</v>
       </c>
       <c r="D23" s="8">
         <v>232503</v>
@@ -10370,10 +10272,10 @@
         <v>293</v>
       </c>
       <c r="I23" t="s">
-        <v>771</v>
+        <v>761</v>
       </c>
       <c r="J23" t="s">
-        <v>772</v>
+        <v>762</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -10384,7 +10286,7 @@
         <v>444</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>788</v>
+        <v>778</v>
       </c>
       <c r="D24" s="8">
         <v>28972</v>
@@ -10396,7 +10298,7 @@
         <v>293</v>
       </c>
       <c r="I24" t="s">
-        <v>759</v>
+        <v>749</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -10407,7 +10309,7 @@
         <v>364</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>763</v>
+        <v>753</v>
       </c>
       <c r="D25" s="12">
         <v>137274</v>
@@ -10422,10 +10324,10 @@
         <v>1928</v>
       </c>
       <c r="I25" s="29" t="s">
-        <v>774</v>
+        <v>764</v>
       </c>
       <c r="J25" t="s">
-        <v>773</v>
+        <v>763</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -10436,7 +10338,7 @@
         <v>447</v>
       </c>
       <c r="C26" s="31" t="s">
-        <v>750</v>
+        <v>740</v>
       </c>
       <c r="D26" s="12">
         <v>137274</v>
@@ -10448,13 +10350,13 @@
         <v>293</v>
       </c>
       <c r="H26" s="41" t="s">
-        <v>749</v>
+        <v>739</v>
       </c>
       <c r="I26" s="29" t="s">
-        <v>777</v>
+        <v>767</v>
       </c>
       <c r="J26" s="29" t="s">
-        <v>747</v>
+        <v>737</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -10465,7 +10367,7 @@
         <v>448</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>750</v>
+        <v>740</v>
       </c>
       <c r="D27" s="12">
         <v>137274</v>
@@ -10477,24 +10379,24 @@
         <v>293</v>
       </c>
       <c r="H27" s="41" t="s">
-        <v>748</v>
+        <v>738</v>
       </c>
       <c r="I27" s="29" t="s">
-        <v>777</v>
+        <v>767</v>
       </c>
       <c r="J27" s="29" t="s">
-        <v>747</v>
+        <v>737</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>751</v>
+        <v>741</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>752</v>
+        <v>742</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>782</v>
+        <v>772</v>
       </c>
       <c r="D28" s="8">
         <v>2577563</v>
@@ -10509,10 +10411,10 @@
         <v>1900</v>
       </c>
       <c r="I28" s="44" t="s">
-        <v>783</v>
+        <v>773</v>
       </c>
       <c r="J28" t="s">
-        <v>784</v>
+        <v>774</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -10523,7 +10425,7 @@
         <v>450</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>737</v>
+        <v>727</v>
       </c>
       <c r="D29" s="8">
         <v>2577563</v>
@@ -10538,10 +10440,10 @@
         <v>1900</v>
       </c>
       <c r="I29" s="44" t="s">
-        <v>783</v>
+        <v>773</v>
       </c>
       <c r="J29" t="s">
-        <v>784</v>
+        <v>774</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -10570,7 +10472,7 @@
         <v>454</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>738</v>
+        <v>728</v>
       </c>
       <c r="D31" s="8">
         <v>634025</v>
@@ -10585,10 +10487,10 @@
         <v>1947</v>
       </c>
       <c r="I31" s="29" t="s">
-        <v>780</v>
+        <v>770</v>
       </c>
       <c r="J31" t="s">
-        <v>781</v>
+        <v>771</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -10809,10 +10711,10 @@
     </row>
     <row r="44" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="35" t="s">
-        <v>671</v>
+        <v>661</v>
       </c>
       <c r="B44" s="35" t="s">
-        <v>671</v>
+        <v>661</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="36">
@@ -10820,7 +10722,7 @@
       </c>
       <c r="E44" s="4"/>
       <c r="F44" s="4" t="s">
-        <v>672</v>
+        <v>662</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -10831,7 +10733,7 @@
         <v>313</v>
       </c>
       <c r="C45" s="29" t="s">
-        <v>739</v>
+        <v>729</v>
       </c>
       <c r="E45" t="s">
         <v>314</v>
@@ -10843,10 +10745,10 @@
         <v>2009</v>
       </c>
       <c r="I45" s="29" t="s">
-        <v>778</v>
+        <v>768</v>
       </c>
       <c r="J45" t="s">
-        <v>779</v>
+        <v>769</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="225" x14ac:dyDescent="0.2">
@@ -10857,7 +10759,7 @@
         <v>315</v>
       </c>
       <c r="C46" s="17" t="s">
-        <v>740</v>
+        <v>730</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>316</v>
@@ -10877,7 +10779,7 @@
         <v>317</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>765</v>
+        <v>755</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>318</v>
@@ -10886,10 +10788,10 @@
         <v>293</v>
       </c>
       <c r="I47" s="29" t="s">
-        <v>775</v>
+        <v>765</v>
       </c>
       <c r="J47" s="29" t="s">
-        <v>776</v>
+        <v>766</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -10900,7 +10802,7 @@
         <v>319</v>
       </c>
       <c r="C48" s="29" t="s">
-        <v>766</v>
+        <v>756</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>318</v>
@@ -10909,7 +10811,7 @@
         <v>293</v>
       </c>
       <c r="I48" s="29" t="s">
-        <v>766</v>
+        <v>756</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -11050,7 +10952,7 @@
         <v>335</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>673</v>
+        <v>663</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
@@ -11068,7 +10970,7 @@
         <v>335</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>674</v>
+        <v>664</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
@@ -11205,7 +11107,7 @@
         <v>471</v>
       </c>
       <c r="C66" s="31" t="s">
-        <v>764</v>
+        <v>754</v>
       </c>
       <c r="D66" s="25">
         <v>274</v>
@@ -11217,10 +11119,10 @@
         <v>358</v>
       </c>
       <c r="I66" s="31" t="s">
-        <v>754</v>
+        <v>744</v>
       </c>
       <c r="J66" t="s">
-        <v>772</v>
+        <v>762</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="16" x14ac:dyDescent="0.2">
@@ -11231,7 +11133,7 @@
         <v>472</v>
       </c>
       <c r="C67" s="29" t="s">
-        <v>763</v>
+        <v>753</v>
       </c>
       <c r="D67" s="25">
         <v>5741</v>
@@ -11251,7 +11153,7 @@
         <v>507</v>
       </c>
       <c r="C68" s="29" t="s">
-        <v>736</v>
+        <v>726</v>
       </c>
       <c r="D68" s="25">
         <v>7731871</v>
@@ -11266,10 +11168,10 @@
         <v>1981</v>
       </c>
       <c r="I68" s="29" t="s">
-        <v>767</v>
+        <v>757</v>
       </c>
       <c r="J68" t="s">
-        <v>784</v>
+        <v>774</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
@@ -11649,10 +11551,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W1"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="E4" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11726,6 +11628,68 @@
       </c>
       <c r="W1" s="1" t="s">
         <v>534</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>854</v>
+      </c>
+      <c r="B4" t="s">
+        <v>512</v>
+      </c>
+      <c r="C4" t="s">
+        <v>626</v>
+      </c>
+      <c r="D4" t="s">
+        <v>855</v>
+      </c>
+      <c r="E4" t="s">
+        <v>831</v>
+      </c>
+      <c r="F4" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>856</v>
+      </c>
+      <c r="B5" t="s">
+        <v>625</v>
+      </c>
+      <c r="C5" t="s">
+        <v>627</v>
+      </c>
+      <c r="E5" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>857</v>
+      </c>
+      <c r="B6" t="s">
+        <v>625</v>
+      </c>
+      <c r="C6" t="s">
+        <v>627</v>
+      </c>
+      <c r="E6" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>858</v>
+      </c>
+      <c r="B7" t="s">
+        <v>625</v>
+      </c>
+      <c r="C7" t="s">
+        <v>627</v>
+      </c>
+      <c r="E7" t="s">
+        <v>628</v>
       </c>
     </row>
   </sheetData>
@@ -11758,7 +11722,7 @@
         <v>537</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>670</v>
+        <v>660</v>
       </c>
       <c r="E1" t="s">
         <v>538</v>
@@ -11890,10 +11854,10 @@
         <v>291</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>803</v>
+        <v>793</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>743</v>
+        <v>733</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="8">
@@ -11905,10 +11869,10 @@
     </row>
     <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>666</v>
+        <v>656</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>795</v>
+        <v>785</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="34">
@@ -11923,10 +11887,10 @@
     </row>
     <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>730</v>
+        <v>720</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>731</v>
+        <v>721</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="34">
@@ -11963,7 +11927,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11:XFD11"/>
@@ -11971,7 +11935,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>616</v>
       </c>
@@ -11982,19 +11946,19 @@
         <v>512</v>
       </c>
       <c r="D1" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
       <c r="E1" t="s">
-        <v>840</v>
+        <v>830</v>
       </c>
       <c r="F1" t="s">
-        <v>841</v>
+        <v>831</v>
       </c>
       <c r="G1" t="s">
         <v>624</v>
       </c>
       <c r="H1" t="s">
-        <v>653</v>
+        <v>643</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -12005,16 +11969,16 @@
         <v>619</v>
       </c>
       <c r="C2" t="s">
-        <v>836</v>
+        <v>826</v>
       </c>
       <c r="D2" t="s">
-        <v>837</v>
+        <v>827</v>
       </c>
       <c r="E2" t="s">
-        <v>838</v>
+        <v>828</v>
       </c>
       <c r="F2" t="s">
-        <v>839</v>
+        <v>829</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -12025,161 +11989,116 @@
         <v>620</v>
       </c>
       <c r="C3" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
-        <v>626</v>
+      <c r="A4" t="s">
+        <v>629</v>
       </c>
       <c r="B4" t="s">
-        <v>625</v>
-      </c>
-      <c r="C4" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
-        <v>652</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>628</v>
+        <v>629</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>631</v>
+      </c>
+      <c r="B5" t="s">
+        <v>630</v>
       </c>
       <c r="C5" t="s">
-        <v>627</v>
-      </c>
-      <c r="G5" s="31" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>632</v>
+        <v>825</v>
+      </c>
+      <c r="D5" t="s">
+        <v>827</v>
+      </c>
+      <c r="E5" t="s">
+        <v>828</v>
+      </c>
+      <c r="F5" t="s">
+        <v>829</v>
+      </c>
+      <c r="H5" s="32" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="37" t="s">
+        <v>797</v>
       </c>
       <c r="B6" t="s">
-        <v>631</v>
+        <v>805</v>
       </c>
       <c r="C6" t="s">
-        <v>627</v>
-      </c>
-      <c r="D6" t="s">
-        <v>634</v>
-      </c>
-      <c r="F6" t="s">
-        <v>635</v>
-      </c>
-      <c r="G6" s="31" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>636</v>
+        <v>796</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="37" t="s">
+        <v>832</v>
       </c>
       <c r="B7" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>638</v>
+        <v>798</v>
+      </c>
+      <c r="C7" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="37" t="s">
+        <v>806</v>
       </c>
       <c r="B8" t="s">
-        <v>637</v>
-      </c>
-      <c r="C8" t="s">
-        <v>835</v>
-      </c>
-      <c r="D8" t="s">
-        <v>837</v>
-      </c>
-      <c r="E8" t="s">
-        <v>838</v>
-      </c>
-      <c r="F8" t="s">
-        <v>839</v>
-      </c>
-      <c r="H8" s="32" t="s">
-        <v>654</v>
+        <v>807</v>
+      </c>
+      <c r="G8" s="29" t="s">
+        <v>804</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="37" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="B9" t="s">
-        <v>815</v>
-      </c>
-      <c r="C9" t="s">
-        <v>806</v>
+        <v>810</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>811</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>843</v>
+        <v>808</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="37" t="s">
-        <v>842</v>
+        <v>816</v>
       </c>
       <c r="B10" t="s">
-        <v>808</v>
+        <v>817</v>
       </c>
       <c r="C10" t="s">
-        <v>813</v>
+        <v>22</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>812</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="37" t="s">
-        <v>816</v>
-      </c>
-      <c r="B11" t="s">
-        <v>817</v>
+        <v>819</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>820</v>
+      </c>
+      <c r="C11" t="s">
+        <v>821</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A12" s="37" t="s">
-        <v>819</v>
-      </c>
-      <c r="B12" t="s">
-        <v>820</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>821</v>
-      </c>
-      <c r="G12" s="29" t="s">
         <v>818</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A13" s="37" t="s">
-        <v>826</v>
-      </c>
-      <c r="B13" t="s">
-        <v>827</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>822</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.2">
-      <c r="A14" s="37" t="s">
-        <v>829</v>
-      </c>
-      <c r="B14" s="37" t="s">
-        <v>830</v>
-      </c>
-      <c r="C14" t="s">
-        <v>831</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>828</v>
       </c>
     </row>
   </sheetData>
@@ -12207,12 +12126,12 @@
         <v>536</v>
       </c>
       <c r="B1" t="s">
-        <v>667</v>
+        <v>657</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>668</v>
+        <v>658</v>
       </c>
       <c r="B2" s="29">
         <v>1960.91</v>
@@ -12220,7 +12139,7 @@
     </row>
     <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>669</v>
+        <v>659</v>
       </c>
       <c r="B3" s="33">
         <v>39011882</v>

</xml_diff>